<commit_message>
working on lightlink fw
</commit_message>
<xml_diff>
--- a/1_Hardware/LightLink_V3/ArduinoPinIndex.xlsx
+++ b/1_Hardware/LightLink_V3/ArduinoPinIndex.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trololololol\Documents\Projects\BRZ\1_Hardware\LightLink_V3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trololololol\OneDrive - University of Ottawa\Documents\BRZ\1_Hardware\LightLink_V3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364422A3-60F8-45AC-9D09-48E7F427B462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30B44B5-D470-4566-A012-C15F4B91E886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1530" yWindow="1410" windowWidth="21600" windowHeight="11295" xr2:uid="{F419665D-1B25-4458-ADD2-E57179E98A67}"/>
+    <workbookView xWindow="13714" yWindow="0" windowWidth="13715" windowHeight="14829" xr2:uid="{F419665D-1B25-4458-ADD2-E57179E98A67}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -543,17 +543,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18255E9-B8D8-4B67-9BC3-BF64C50930BF}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.84375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -564,7 +564,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>2</v>
       </c>
@@ -572,7 +572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3">
         <f>A2+1</f>
         <v>3</v>
@@ -581,7 +581,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4">
         <f t="shared" ref="A4:A46" si="0">A3+1</f>
         <v>4</v>
@@ -591,7 +591,7 @@
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -600,7 +600,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -610,7 +610,7 @@
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -619,7 +619,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -629,7 +629,7 @@
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -638,7 +638,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -648,7 +648,7 @@
       </c>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -657,7 +657,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -670,7 +670,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -679,7 +679,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -689,7 +689,7 @@
       </c>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -698,7 +698,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -708,7 +708,7 @@
       </c>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -717,7 +717,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -727,7 +727,7 @@
       </c>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -736,7 +736,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -746,7 +746,7 @@
       </c>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -755,7 +755,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -765,7 +765,7 @@
       </c>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -774,7 +774,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -783,7 +783,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -792,7 +792,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -801,7 +801,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -810,7 +810,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -819,7 +819,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -828,7 +828,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -837,7 +837,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -846,7 +846,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -855,7 +855,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -864,7 +864,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -873,7 +873,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -882,7 +882,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -891,7 +891,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -900,7 +900,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -910,7 +910,7 @@
       </c>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -919,7 +919,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -929,7 +929,7 @@
       </c>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -939,7 +939,7 @@
       </c>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -948,7 +948,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -957,7 +957,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -969,7 +969,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -981,7 +981,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>46</v>

</xml_diff>